<commit_message>
finishing genetics methods section for MS
</commit_message>
<xml_diff>
--- a/protocols/melansonprimerseqs.xlsx
+++ b/protocols/melansonprimerseqs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna1/Documents/UBC/Bombus Project/Microsatellites/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenna1/fv_landscapeforaging/protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD0375E-724E-2045-A26D-CFF72D8CDBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2437D40A-05B3-944D-983A-90B19298F796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="840" windowWidth="16680" windowHeight="16260" activeTab="1" xr2:uid="{1B272F40-BB64-7941-A8BD-F37B192F690B}"/>
+    <workbookView xWindow="42660" yWindow="1120" windowWidth="29920" windowHeight="23920" activeTab="2" xr2:uid="{1B272F40-BB64-7941-A8BD-F37B192F690B}"/>
   </bookViews>
   <sheets>
     <sheet name="mixtus" sheetId="1" r:id="rId1"/>
     <sheet name="impatiens" sheetId="2" r:id="rId2"/>
+    <sheet name="combined" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="178">
   <si>
     <t>BT10</t>
   </si>
@@ -87,9 +88,6 @@
     <t>Dye Tag</t>
   </si>
   <si>
-    <t>Primer Sequence</t>
-  </si>
-  <si>
     <t>TCTTGCTATCCACCACCCGC</t>
   </si>
   <si>
@@ -156,9 +154,6 @@
     <t>NED</t>
   </si>
   <si>
-    <t>Ta</t>
-  </si>
-  <si>
     <t>TCTTCTGCTCCTTTCTCCATTC</t>
   </si>
   <si>
@@ -207,9 +202,6 @@
     <t>ACTCCGTTATTCCCTTTCTCCT</t>
   </si>
   <si>
-    <t>Reverse</t>
-  </si>
-  <si>
     <t>Plex</t>
   </si>
   <si>
@@ -354,9 +346,6 @@
     <t>335-365</t>
   </si>
   <si>
-    <t>added 'C' base to 5' end to avoid quenching 6FAM</t>
-  </si>
-  <si>
     <t>BTMS0073</t>
   </si>
   <si>
@@ -379,13 +368,637 @@
   </si>
   <si>
     <t>AGGGACACGCGAACAGAC</t>
+  </si>
+  <si>
+    <t>Size Range</t>
+  </si>
+  <si>
+    <t>119-157</t>
+  </si>
+  <si>
+    <t>236-278</t>
+  </si>
+  <si>
+    <t>339-367</t>
+  </si>
+  <si>
+    <t>137-173</t>
+  </si>
+  <si>
+    <t>292-320</t>
+  </si>
+  <si>
+    <t>148-184</t>
+  </si>
+  <si>
+    <t>230-330</t>
+  </si>
+  <si>
+    <t>142-200</t>
+  </si>
+  <si>
+    <t>101-151</t>
+  </si>
+  <si>
+    <t>233-303</t>
+  </si>
+  <si>
+    <t>106-136</t>
+  </si>
+  <si>
+    <t>173-206</t>
+  </si>
+  <si>
+    <t>184-256</t>
+  </si>
+  <si>
+    <t>276-320</t>
+  </si>
+  <si>
+    <t>112-136</t>
+  </si>
+  <si>
+    <t>177-207</t>
+  </si>
+  <si>
+    <t>Forward Sequence</t>
+  </si>
+  <si>
+    <t>Reverse Sequence</t>
+  </si>
+  <si>
+    <t>Ta-f</t>
+  </si>
+  <si>
+    <t>Ta-r</t>
+  </si>
+  <si>
+    <t>Ta-reverse</t>
+  </si>
+  <si>
+    <t>Ta-forward</t>
+  </si>
+  <si>
+    <t>128-172</t>
+  </si>
+  <si>
+    <t>266-268</t>
+  </si>
+  <si>
+    <t>116-136</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>266-277</t>
+  </si>
+  <si>
+    <t>113-197</t>
+  </si>
+  <si>
+    <t>229-289</t>
+  </si>
+  <si>
+    <t>154-196</t>
+  </si>
+  <si>
+    <t>104-120</t>
+  </si>
+  <si>
+    <t>163-195</t>
+  </si>
+  <si>
+    <t>342-362</t>
+  </si>
+  <si>
+    <t>124-172</t>
+  </si>
+  <si>
+    <t>158-214</t>
+  </si>
+  <si>
+    <t>266-304</t>
+  </si>
+  <si>
+    <t>143-151</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>B. mixtus</t>
+  </si>
+  <si>
+    <t>B. impatiens</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Maintained</t>
+  </si>
+  <si>
+    <t>Rarefied Allelic Richness</t>
+  </si>
+  <si>
+    <t>no (F_is)</t>
+  </si>
+  <si>
+    <t>no (error rate)</t>
+  </si>
+  <si>
+    <t>no (LD)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGACAGAAGCATAGACGCACCG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CTGTCGCATTATTCGCGGTT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGAGCAAGAGGGCTAGACAAAAG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCGAGTACGTGTACGTGTTCTATG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGCTAGGAAAGATTAGCACTACC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CACCGGCATTTTACACACCA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCCAACTACGTTCAATATCG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCTTGCTGGTGAATTGTGC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGGAGATGGATATAGATGAG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AGAGAAATTGCATGCGGTCG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAGGATAGGGTAGGTAAGCAG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GATCGTAATGACTCGATATG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CGTTTATCTGCTTCTCTCGTTCG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCAACAGGTCGGGTTAGAG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CAGCAACAGTCACAACAAACGC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGGAGAGAAAGACCAAG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTAGCATGCTCTCCGTGTTG</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AGGGACACGCGAACAGAC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GGTGATCGCTTAAAGCTC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TTCGAAGCCTCGATGTCGT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCCTCTGTGTGTTCTCTTACTTGGC</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -427,6 +1040,36 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -448,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -458,6 +1101,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,109 +1418,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C807CCEB-818F-9245-A747-FE8CC7461017}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L4"/>
+      <selection activeCell="E16" sqref="E16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G2">
+        <v>55.9</v>
+      </c>
+      <c r="H2">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2">
-        <v>54.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>55.9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3">
+        <v>54.8</v>
+      </c>
+      <c r="H3">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -883,56 +1538,62 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="G4">
-        <v>54.8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>56.5</v>
+      </c>
+      <c r="H4">
+        <v>55.6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G5">
-        <v>51.9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5">
-        <v>55.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>56.2</v>
+      </c>
+      <c r="H5">
+        <v>56.3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -941,346 +1602,350 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="G6">
-        <v>56.5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6">
-        <v>55.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>56.3</v>
+      </c>
+      <c r="H6">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7">
+        <v>59.8</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
-      </c>
-      <c r="G7">
-        <v>49.4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7">
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G8">
-        <v>56.2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8">
+        <v>56.1</v>
+      </c>
+      <c r="H8">
         <v>56.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G9">
-        <v>52.3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9">
-        <v>57.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="H9">
+        <v>54.4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>56.3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>51.9</v>
+      </c>
+      <c r="H10">
+        <v>55.3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G11">
+        <v>52.3</v>
+      </c>
+      <c r="H11">
+        <v>57.2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12">
         <v>55</v>
       </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11">
+      <c r="H12">
         <v>56.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12">
-        <v>59.8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="G13">
         <v>57.3</v>
       </c>
-      <c r="H13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13">
+      <c r="H13">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G14">
         <v>56.3</v>
       </c>
-      <c r="H14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14">
+      <c r="H14">
         <v>54.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>50.7</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <v>51.3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="I15">
-        <v>51.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
       <c r="G16">
-        <v>56.1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16">
-        <v>56.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17">
         <v>59.4</v>
       </c>
-      <c r="H17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17">
+      <c r="H16">
         <v>55.4</v>
       </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
-    <sortCondition descending="1" ref="B1:B24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
+    <sortCondition ref="C2:C16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1288,49 +1953,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD7D5FF-843C-0548-AF23-7ED670C444DA}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="4" max="5" width="27.5" customWidth="1"/>
     <col min="6" max="6" width="30.1640625" customWidth="1"/>
-    <col min="8" max="8" width="28.5" customWidth="1"/>
+    <col min="9" max="9" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1338,31 +2006,34 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>51.9</v>
       </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2">
+      <c r="H2">
         <v>55.3</v>
       </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1370,31 +2041,34 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G3">
         <v>49.4</v>
       </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3">
+      <c r="H3">
         <v>47.5</v>
       </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="K3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1402,31 +2076,34 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G4">
         <v>52.3</v>
       </c>
-      <c r="H4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4">
+      <c r="H4">
         <v>57.2</v>
       </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="K4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1434,31 +2111,34 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G5">
         <v>53</v>
       </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5">
+      <c r="H5">
         <v>54.4</v>
       </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1466,31 +2146,34 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G6">
         <v>59.8</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6">
+      <c r="H6">
         <v>60</v>
       </c>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1498,28 +2181,31 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="G7">
         <v>56.3</v>
       </c>
-      <c r="H7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7">
+      <c r="H7">
         <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1527,295 +2213,321 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G8">
         <v>56.3</v>
       </c>
-      <c r="H8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8">
+      <c r="H8">
         <v>54.8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
         <v>109</v>
       </c>
-      <c r="E9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" t="s">
-        <v>113</v>
+      <c r="J9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>54.8</v>
+      </c>
+      <c r="H10">
+        <v>56</v>
+      </c>
+      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11">
-        <v>54.8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11">
-        <v>56</v>
+        <v>85</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>77</v>
+        <v>126</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>74</v>
+      </c>
+      <c r="K12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>77</v>
+        <v>120</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="I13" t="s">
+        <v>88</v>
+      </c>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>74</v>
+      </c>
+      <c r="K13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
-        <v>91</v>
+        <v>122</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>74</v>
       </c>
       <c r="K14" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>77</v>
+        <v>119</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>57.3</v>
+      </c>
+      <c r="H15">
+        <v>57.6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>74</v>
+      </c>
+      <c r="K15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G16">
-        <v>57.3</v>
-      </c>
-      <c r="H16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16">
-        <v>57.6</v>
+        <v>55</v>
+      </c>
+      <c r="H16">
+        <v>56.4</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="K16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17">
-        <v>55</v>
-      </c>
-      <c r="H17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17">
-        <v>56.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="J17" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1824,9 +2536,8 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1835,9 +2546,8 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1846,9 +2556,8 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1857,42 +2566,38 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1901,9 +2606,8 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1912,26 +2616,1093 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J30">
+    <sortCondition ref="C2:C30"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB953491-3BE7-5D4D-A35E-8C997CB9BC48}">
+  <dimension ref="A1:O43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5">
+        <v>14.6</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8">
+        <v>26.9</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D9" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11">
+        <v>34.9</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13">
+        <v>27.8</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D15" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="9">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D19" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19">
+        <v>17.5</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D21" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21">
+        <v>8.9</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D23" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25">
+        <v>15.9</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D27" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F27">
+        <v>8.9</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28">
+        <v>18</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="D29" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+      <c r="D31" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31">
+        <v>18</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D33" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33">
+        <v>6.8</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D35" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35">
+        <v>22.5</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D37" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37">
+        <v>10.7</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D39" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D41" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41">
+        <v>19.8</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D43" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43">
+        <v>7.9</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
-    <sortCondition ref="C2:C31"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>